<commit_message>
Added fat jar creation plugin in pom.xml
</commit_message>
<xml_diff>
--- a/input-sample.xlsx
+++ b/input-sample.xlsx
@@ -16,17 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
-  <si>
-    <t>Key</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Mapping_Source</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -34,9 +28,6 @@
   </si>
   <si>
     <t>C3</t>
-  </si>
-  <si>
-    <t>Mapping_Target</t>
   </si>
   <si>
     <t>C3_Target</t>
@@ -101,11 +92,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="mm\-dd\-yyyy"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="mm\-dd\-yyyy"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -128,14 +119,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,37 +158,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,7 +211,45 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -236,36 +257,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,187 +271,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,6 +462,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -485,21 +491,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -537,17 +528,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -571,18 +551,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -592,130 +583,130 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -724,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,48 +1035,39 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD3"/>
+      <selection activeCell="A1" sqref="A$1:A$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="12.5" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="12.5" outlineLevelRow="2" outlineLevelCol="2"/>
   <sheetData>
-    <row r="1" s="2" customFormat="1" ht="15.75" customHeight="1" spans="1:2">
+    <row r="1" s="2" customFormat="1" ht="15.75" customHeight="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" s="1" customFormat="1" ht="15.75" customHeight="1" spans="1:3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A2" s="3" t="s">
+    <row r="3" ht="15.75" customHeight="1" spans="1:3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1110,69 +1092,69 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" customHeight="1" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1197,60 +1179,60 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Duplicate and Unique Data finder method
</commit_message>
<xml_diff>
--- a/input-sample.xlsx
+++ b/input-sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7070"/>
+    <workbookView windowWidth="19200" windowHeight="7070" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mapping" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Y</t>
   </si>
@@ -60,9 +60,6 @@
     <t>yy</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
   </si>
   <si>
     <t>O</t>
-  </si>
-  <si>
-    <t>B1</t>
   </si>
   <si>
     <t>P1</t>
@@ -92,11 +86,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="mm\-dd\-yyyy"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="mm\-dd\-yyyy"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -114,51 +108,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -172,9 +121,54 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -186,9 +180,69 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,66 +255,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -271,19 +265,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,19 +385,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,139 +433,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -462,6 +456,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -498,8 +501,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -521,39 +539,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -562,151 +547,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -715,7 +709,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1037,7 +1031,7 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A$1:A$1048576"/>
     </sheetView>
   </sheetViews>
@@ -1082,7 +1076,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="4" outlineLevelCol="3"/>
@@ -1134,27 +1128,27 @@
     </row>
     <row r="4" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" customHeight="1" spans="1:3">
       <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1168,8 +1162,8 @@
   <sheetPr/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="4" outlineLevelCol="3"/>
@@ -1196,7 +1190,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -1204,7 +1198,7 @@
     </row>
     <row r="3" customHeight="1" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
@@ -1215,24 +1209,24 @@
     </row>
     <row r="4" customHeight="1" spans="1:3">
       <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>